<commit_message>
Added Plotting in Univariable Analyisis
</commit_message>
<xml_diff>
--- a/_dataset/Data_Dictionary.xlsx
+++ b/_dataset/Data_Dictionary.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohit/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dicotips/workspace/LJMU/Module04a/LendingClubCaseStudy/_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0B6461-17AA-CE4B-B7E0-ADAEDF093552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="17920" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
     <sheet name="RejectStats" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$116</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -779,7 +780,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -941,7 +942,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1124,6 +1125,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1362,7 +1369,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1396,6 +1403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="92">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1516,7 +1524,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1818,15 +1826,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1863,7 +1871,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -1881,8 +1889,8 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1944,7 +1952,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>165</v>
       </c>
@@ -1953,7 +1961,7 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>100</v>
       </c>
@@ -1962,7 +1970,7 @@
       </c>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -1980,7 +1988,7 @@
       </c>
       <c r="C16" s="20"/>
     </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1990,7 +1998,7 @@
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2007,7 +2015,7 @@
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -2016,8 +2024,8 @@
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -2025,7 +2033,7 @@
       </c>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>154</v>
       </c>
@@ -2034,7 +2042,7 @@
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
@@ -2043,7 +2051,7 @@
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2052,7 +2060,7 @@
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
@@ -2061,7 +2069,7 @@
       </c>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
@@ -2070,8 +2078,8 @@
       </c>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2079,8 +2087,8 @@
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="21" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2088,7 +2096,7 @@
       </c>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
@@ -2133,7 +2141,7 @@
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>26</v>
       </c>
@@ -2142,7 +2150,7 @@
       </c>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -2151,8 +2159,8 @@
       </c>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2160,8 +2168,8 @@
       </c>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="21" t="s">
         <v>13</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2171,7 +2179,7 @@
       <c r="I37" s="10"/>
       <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -2180,7 +2188,7 @@
       </c>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>46</v>
       </c>
@@ -2189,7 +2197,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>47</v>
       </c>
@@ -2207,7 +2215,7 @@
       </c>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
@@ -2217,7 +2225,7 @@
       <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="21" t="s">
         <v>2</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -2225,7 +2233,7 @@
       </c>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -2243,7 +2251,7 @@
       </c>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>1</v>
       </c>
@@ -2306,7 +2314,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>27</v>
       </c>
@@ -2324,7 +2332,7 @@
       </c>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>28</v>
       </c>
@@ -2378,7 +2386,7 @@
       </c>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>44</v>
       </c>
@@ -2502,7 +2510,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>29</v>
       </c>
@@ -2558,7 +2566,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>35</v>
       </c>
@@ -2566,7 +2574,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>36</v>
       </c>
@@ -2590,7 +2598,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>123</v>
       </c>
@@ -2598,7 +2606,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>30</v>
       </c>
@@ -2614,15 +2622,15 @@
         <v>146</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
+    <row r="89" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>15</v>
       </c>
@@ -2630,7 +2638,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
         <v>164</v>
       </c>
@@ -2638,7 +2646,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>31</v>
       </c>
@@ -2646,7 +2654,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>32</v>
       </c>
@@ -2654,8 +2662,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
+    <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="21" t="s">
         <v>9</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -2670,15 +2678,15 @@
         <v>147</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
+    <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" s="21" t="s">
         <v>5</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>19</v>
       </c>
@@ -2710,7 +2718,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>33</v>
       </c>
@@ -2758,7 +2766,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>37</v>
       </c>
@@ -2766,7 +2774,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>38</v>
       </c>
@@ -2774,7 +2782,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>40</v>
       </c>
@@ -2782,7 +2790,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>41</v>
       </c>
@@ -2790,7 +2798,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>39</v>
       </c>
@@ -2806,7 +2814,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>16</v>
       </c>
@@ -2814,8 +2822,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="7" t="s">
+    <row r="114" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A114" s="21" t="s">
         <v>232</v>
       </c>
       <c r="B114" s="2" t="s">
@@ -2838,18 +2846,14 @@
         <v>183</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B118" s="13" t="s">
         <v>156</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B57">
-    <sortState ref="A2:B116">
-      <sortCondition ref="A1:A116"/>
-    </sortState>
-  </autoFilter>
-  <sortState ref="A2:B101">
+  <autoFilter ref="A1:B116" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B101">
     <sortCondition ref="A2:A101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2858,7 +2862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2895,7 +2899,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>169</v>
       </c>
@@ -2911,7 +2915,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>170</v>
       </c>
@@ -2943,7 +2947,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>173</v>
       </c>
@@ -2960,7 +2964,7 @@
       <c r="B12" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B10"/>
+  <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0"/>
 </worksheet>

</xml_diff>